<commit_message>
Solved and updated with Create Query and Constant class
</commit_message>
<xml_diff>
--- a/src/main/resources/StudentMarks.xlsx
+++ b/src/main/resources/StudentMarks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/368216efa4f12ee9/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\JAVA\dataconversion\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CBF7183-35F9-4983-BDD1-44F66D4194EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A6940D-BA8E-4974-BF31-24D7A59FD9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB39CE70-1757-4CC1-8D82-439C1D488CA8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Dinesh</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Venky</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Marks</t>
   </si>
 </sst>
 </file>
@@ -55,7 +61,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -65,6 +71,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -96,9 +108,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -415,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418A2D89-9B78-44C3-B75A-2721D2988978}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,43 +442,51 @@
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B2" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:2" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>100</v>
       </c>
     </row>

</xml_diff>